<commit_message>
Update Dataset variables explainer.xlsx
</commit_message>
<xml_diff>
--- a/Dataset variables explainer.xlsx
+++ b/Dataset variables explainer.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rheerema\Documents\MATLAB\MoodChoicePhysiology2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roeland\Documents\MATLAB\MoodChoicePhysiology2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D3CE59-E3B6-4E51-94D0-2C5254A40672}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="9510" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="AllData.trialinfo" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
   <si>
     <t>induction</t>
   </si>
@@ -546,11 +545,17 @@
   <si>
     <t>numbers of the samples where the gaze was labelled as focused on the right cost</t>
   </si>
+  <si>
+    <t>ind_trialno</t>
+  </si>
+  <si>
+    <t>Choice trial number following the most recent emotion induction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -895,11 +900,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,113 +939,121 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1051,7 +1064,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1074,7 +1087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1173,7 +1186,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1226,7 +1239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1523FF84-EF0A-41D7-90ED-8218508EF1CD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1295,7 +1308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D764A8D7-8CAD-4E8A-A1F4-926388DCFEE1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1364,10 +1377,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{361B5718-7A18-4001-8B7C-7EBB28C055D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1431,7 +1444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6F72F0-B772-434A-BA47-18889444E773}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1524,7 +1537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FDEF0D-6EC1-4724-910B-A901FC66F941}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">

</xml_diff>